<commit_message>
[MacOS Only! ]Add Packing scripts, fix folder path on MacOS, fix assess record, code cleaning
[FATAL!]Please modify tools/FileManager.py if you want to run this file in python command line. Otherwise this version of code could only work after compiled into macos .app format.
</commit_message>
<xml_diff>
--- a/database/import.xlsx
+++ b/database/import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\design_tool_v3\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/centaurus/Code/doc_automation/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF616052-75A6-4AD6-9202-794DC8D88867}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B8B509-ABFE-634E-994F-F508B0F776DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5373" yWindow="1101" windowWidth="17425" windowHeight="8955" xr2:uid="{4368B5D2-669C-4275-82E9-FEC59B79763E}"/>
+    <workbookView xWindow="5380" yWindow="1100" windowWidth="17420" windowHeight="8960" xr2:uid="{4368B5D2-669C-4275-82E9-FEC59B79763E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>学号</t>
   </si>
@@ -60,18 +60,6 @@
     <t>无</t>
   </si>
   <si>
-    <t>王老师1</t>
-  </si>
-  <si>
-    <t>王老师2</t>
-  </si>
-  <si>
-    <t>王老师3</t>
-  </si>
-  <si>
-    <t>王老师4</t>
-  </si>
-  <si>
     <t>标题1</t>
   </si>
   <si>
@@ -114,21 +102,6 @@
     <t>学院a4</t>
   </si>
   <si>
-    <t>张1</t>
-  </si>
-  <si>
-    <t>张2</t>
-  </si>
-  <si>
-    <t>张3</t>
-  </si>
-  <si>
-    <t>张4</t>
-  </si>
-  <si>
-    <t>张5</t>
-  </si>
-  <si>
     <t>学院a5</t>
   </si>
   <si>
@@ -144,7 +117,22 @@
     <t>标题5</t>
   </si>
   <si>
-    <t>王老师5</t>
+    <t>zhangsan</t>
+  </si>
+  <si>
+    <t>深深的</t>
+  </si>
+  <si>
+    <t>得到的</t>
+  </si>
+  <si>
+    <t>猜猜猜</t>
+  </si>
+  <si>
+    <t>从吃</t>
+  </si>
+  <si>
+    <t>王老师</t>
   </si>
 </sst>
 </file>
@@ -155,13 +143,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -190,7 +178,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -206,7 +194,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -505,12 +493,12 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H2" sqref="H2:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.95" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -539,146 +527,146 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>114514</v>
+        <v>2020211033376</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1223445</v>
+        <v>2020211033378</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="I3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>4445</v>
+        <v>2020211023021</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1212</v>
+        <v>2020211023022</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="I5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1211</v>
+        <v>2020211023023</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
         <v>35</v>
-      </c>
-      <c r="E6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" t="s">
-        <v>39</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>

</xml_diff>